<commit_message>
preparando el sprint II
</commit_message>
<xml_diff>
--- a/encabezados_y_calendario.xlsx
+++ b/encabezados_y_calendario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0eaf3dded534d368/Desktop/Data_Analytics/PROYECTOS/proyecto-da-promo-F-modulo-2-team-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="381" documentId="8_{24825327-74E0-4170-8EF1-8CAB6C218DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A27D6B8E-B441-4A5F-A44B-6BEE52A9C71F}"/>
+  <xr:revisionPtr revIDLastSave="409" documentId="8_{24825327-74E0-4170-8EF1-8CAB6C218DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18CE4F7B-64E1-45E1-BD49-C3CC17588104}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9EDE54BF-6961-4DE8-8847-425C4F85DDE6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{9EDE54BF-6961-4DE8-8847-425C4F85DDE6}"/>
   </bookViews>
   <sheets>
     <sheet name="calendario_ppt" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
   <si>
     <t>Fase I</t>
   </si>
@@ -523,6 +523,9 @@
   </si>
   <si>
     <t>función para buscar todos los archivos que coincidan con ese patrón</t>
+  </si>
+  <si>
+    <t>limpieza código</t>
   </si>
 </sst>
 </file>
@@ -744,7 +747,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -890,16 +893,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -964,9 +975,6 @@
     <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1025,6 +1033,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1054,15 +1065,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>534866</xdr:colOff>
+      <xdr:colOff>586153</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>139210</xdr:rowOff>
+      <xdr:rowOff>73269</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>7327</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>65941</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>21980</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>65942</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1077,8 +1088,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1751135" y="1091710"/>
-          <a:ext cx="6433038" cy="2212731"/>
+          <a:off x="1802422" y="1025769"/>
+          <a:ext cx="7085135" cy="2469173"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1164,6 +1175,64 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>359019</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>51289</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>549519</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>102577</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Left Brace 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B5F4785-3347-139B-4663-3C28AFCACE1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="359019" y="2908789"/>
+          <a:ext cx="190500" cy="1575288"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1472,8 +1541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E75B13F-2F6B-47C3-89BC-BF712B9E1F87}">
   <dimension ref="B4:AF17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,314 +1555,324 @@
     <col min="33" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="Q6" s="4"/>
-    </row>
-    <row r="7" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="Q7" s="47" t="s">
+    <row r="4" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q7" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="48"/>
-      <c r="S7" s="48"/>
-      <c r="T7" s="48"/>
-      <c r="U7" s="48"/>
-      <c r="V7" s="48"/>
-      <c r="W7" s="48"/>
-      <c r="X7" s="48"/>
-      <c r="Y7" s="48"/>
-      <c r="Z7" s="48"/>
-      <c r="AA7" s="48"/>
-      <c r="AB7" s="48"/>
-      <c r="AC7" s="48"/>
-      <c r="AD7" s="48"/>
-      <c r="AE7" s="48"/>
-      <c r="AF7" s="48"/>
-    </row>
-    <row r="8" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="13" t="s">
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="46"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="46"/>
+      <c r="AB7" s="46"/>
+      <c r="AC7" s="46"/>
+      <c r="AD7" s="46"/>
+      <c r="AE7" s="46"/>
+      <c r="AF7" s="46"/>
+    </row>
+    <row r="8" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="15" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="4" t="s">
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AA8" s="4"/>
-      <c r="AF8" s="5" t="s">
+      <c r="AA8" s="3"/>
+      <c r="AF8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="6">
+    <row r="9" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="5">
         <v>45224</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>45225</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>45226</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>45227</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>45228</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>45229</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>45230</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>45231</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <v>45232</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="5">
         <v>45233</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="5">
         <v>45234</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="5">
         <v>45235</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="5">
         <v>45236</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="6">
         <v>45237</v>
       </c>
-      <c r="R9" s="6">
+      <c r="R9" s="5">
         <v>45238</v>
       </c>
-      <c r="S9" s="6">
+      <c r="S9" s="5">
         <v>45239</v>
       </c>
-      <c r="T9" s="6">
+      <c r="T9" s="5">
         <v>45240</v>
       </c>
-      <c r="U9" s="6">
+      <c r="U9" s="5">
         <v>45241</v>
       </c>
-      <c r="V9" s="6">
+      <c r="V9" s="5">
         <v>45242</v>
       </c>
-      <c r="W9" s="6">
+      <c r="W9" s="5">
         <v>45243</v>
       </c>
-      <c r="X9" s="6">
+      <c r="X9" s="5">
         <v>45244</v>
       </c>
-      <c r="Y9" s="6">
+      <c r="Y9" s="5">
         <v>45245</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="Z9" s="6">
         <v>45246</v>
       </c>
-      <c r="AA9" s="6">
+      <c r="AA9" s="5">
         <v>45247</v>
       </c>
-      <c r="AB9" s="6">
+      <c r="AB9" s="5">
         <v>45248</v>
       </c>
-      <c r="AC9" s="6">
+      <c r="AC9" s="5">
         <v>45249</v>
       </c>
-      <c r="AD9" s="27">
+      <c r="AD9" s="26">
         <v>45250</v>
       </c>
-      <c r="AE9" s="6">
+      <c r="AE9" s="5">
         <v>45251</v>
       </c>
-      <c r="AF9" s="8">
+      <c r="AF9" s="7">
         <v>45252</v>
       </c>
     </row>
-    <row r="10" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="53"/>
-      <c r="Q10" s="25"/>
-      <c r="Z10" s="25"/>
-      <c r="AF10" s="26"/>
-    </row>
-    <row r="11" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="51"/>
+      <c r="Q10" s="24"/>
+      <c r="Z10" s="24"/>
+      <c r="AF10" s="25"/>
+    </row>
+    <row r="11" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="49" t="s">
+      <c r="K11" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50"/>
-      <c r="Q11" s="50"/>
-      <c r="R11" s="50"/>
-      <c r="S11" s="50"/>
-      <c r="T11" s="50"/>
-      <c r="U11" s="50"/>
-      <c r="V11" s="50"/>
-      <c r="W11" s="50"/>
-      <c r="X11" s="50"/>
-      <c r="Y11" s="51"/>
-      <c r="Z11" s="25"/>
-      <c r="AF11" s="26"/>
-    </row>
-    <row r="12" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="48"/>
+      <c r="W11" s="48"/>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="49"/>
+      <c r="Z11" s="24"/>
+      <c r="AF11" s="25"/>
+    </row>
+    <row r="12" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="49" t="s">
+      <c r="K12" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="50"/>
-      <c r="T12" s="50"/>
-      <c r="U12" s="50"/>
-      <c r="V12" s="50"/>
-      <c r="W12" s="50"/>
-      <c r="X12" s="50"/>
-      <c r="Y12" s="51"/>
-      <c r="Z12" s="25"/>
-      <c r="AF12" s="26"/>
-    </row>
-    <row r="13" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="48"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="49"/>
+      <c r="Z12" s="24"/>
+      <c r="AF12" s="25"/>
+    </row>
+    <row r="13" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="54" t="s">
+      <c r="J13" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="55"/>
-      <c r="L13" s="56"/>
-      <c r="Q13" s="25"/>
-      <c r="Z13" s="25"/>
-      <c r="AF13" s="26"/>
-    </row>
-    <row r="14" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
+      <c r="K13" s="53"/>
+      <c r="L13" s="54"/>
+      <c r="Q13" s="24"/>
+      <c r="Z13" s="24"/>
+      <c r="AF13" s="25"/>
+    </row>
+    <row r="14" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q14" s="44" t="s">
+      <c r="Q14" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="R14" s="45"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="45"/>
-      <c r="U14" s="45"/>
-      <c r="V14" s="45"/>
-      <c r="W14" s="46"/>
-      <c r="Z14" s="25"/>
-      <c r="AF14" s="26"/>
-    </row>
-    <row r="15" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="43"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="44"/>
+      <c r="Z14" s="24"/>
+      <c r="AF14" s="25"/>
+    </row>
+    <row r="15" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q15" s="25"/>
-      <c r="X15" s="44" t="s">
+      <c r="Q15" s="24"/>
+      <c r="Y15" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="Y15" s="46"/>
-      <c r="Z15" s="25"/>
-      <c r="AF15" s="26"/>
-    </row>
-    <row r="16" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+      <c r="Z15" s="44"/>
+      <c r="AF15" s="25"/>
+    </row>
+    <row r="16" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q16" s="25"/>
-      <c r="Z16" s="33" t="s">
+      <c r="Q16" s="24"/>
+      <c r="Z16" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="AA16" s="34"/>
-      <c r="AB16" s="34"/>
-      <c r="AC16" s="34"/>
-      <c r="AD16" s="34"/>
-      <c r="AE16" s="35"/>
-      <c r="AF16" s="26"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="2"/>
+      <c r="AA16" s="32"/>
+      <c r="AB16" s="32"/>
+      <c r="AC16" s="32"/>
+      <c r="AD16" s="32"/>
+      <c r="AE16" s="33"/>
+      <c r="AF16" s="25"/>
+    </row>
+    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="24"/>
+      <c r="W17" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="X17" s="43"/>
+      <c r="Y17" s="43"/>
+      <c r="Z17" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="W17:Z17"/>
     <mergeCell ref="Q14:W14"/>
     <mergeCell ref="Q7:AF7"/>
     <mergeCell ref="K11:Y11"/>
     <mergeCell ref="K12:Y12"/>
-    <mergeCell ref="X15:Y15"/>
     <mergeCell ref="D10:L10"/>
     <mergeCell ref="J13:L13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1802,7 +1881,7 @@
   <dimension ref="A3:P22"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1841,271 +1920,271 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="P5" s="29"/>
+      <c r="P5" s="28"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="37" t="s">
+      <c r="M6" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="N6" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="21" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="28" t="s">
+      <c r="L9" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="M9" s="28" t="s">
+      <c r="M9" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="N9" s="28" t="s">
+      <c r="N9" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="K11" s="39" t="s">
+      <c r="K11" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="21" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="40" t="s">
+      <c r="I14" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="18" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="24"/>
+      <c r="B15" s="23"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I16" s="22" t="s">
+      <c r="I16" s="21" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="36" t="s">
+      <c r="K17" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="L17" s="36" t="s">
+      <c r="L17" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="M17" s="36" t="s">
+      <c r="M17" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="N17" s="36" t="s">
+      <c r="N17" s="34" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="58" t="s">
+      <c r="F18" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="58"/>
+      <c r="G18" s="56"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
+      <c r="C19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
+      <c r="C20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="22" t="s">
+      <c r="I21" s="21" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="I22" s="36" t="s">
+      <c r="I22" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="J22" s="36" t="s">
+      <c r="J22" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="K22" s="36" t="s">
+      <c r="K22" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="L22" s="36" t="s">
+      <c r="L22" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="M22" s="36" t="s">
+      <c r="M22" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="O22" s="38" t="s">
+      <c r="O22" s="36" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2122,8 +2201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6956CFFF-5EE3-4C0C-B1A3-2515991C34EC}">
   <dimension ref="B6:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,18 +2213,18 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="41"/>
+      <c r="C7" s="39"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="41" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="43"/>
+      <c r="C9" s="41"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -2153,17 +2232,17 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="40" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2173,11 +2252,11 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -2185,12 +2264,12 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -2198,17 +2277,17 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="38"/>
+      <c r="C20" s="36"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
@@ -2216,15 +2295,15 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
@@ -2232,14 +2311,14 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actualizado para sprint II
</commit_message>
<xml_diff>
--- a/encabezados_y_calendario.xlsx
+++ b/encabezados_y_calendario.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0eaf3dded534d368/Desktop/Data_Analytics/PROYECTOS/proyecto-da-promo-F-modulo-2-team-4/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_AC7327F3DE424B4827B10DF6C8E7AD994704CC89" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50CF9D00-DB88-4EDA-80EB-BEAF76E96F18}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calendario_ppt" sheetId="1" r:id="rId1"/>
     <sheet name="diseño tablas" sheetId="2" r:id="rId2"/>
-    <sheet name="unificar csv" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
   <si>
     <t>Fase I</t>
   </si>
@@ -192,9 +197,6 @@
     <t>Inserción</t>
   </si>
   <si>
-    <t>Diseño BBDD</t>
-  </si>
-  <si>
     <t>Soluciones en base al análisis de datos</t>
   </si>
   <si>
@@ -342,14 +344,6 @@
     <t>premios</t>
   </si>
   <si>
-    <t>limpiar año nac (cuando no tiene año pero sí fecha, copia la ciudad donde nació LOL)</t>
-  </si>
-  <si>
-    <t>limpiar? coje uno de estos
-Awards 45 won 13 nomin
-Won 4 Oscars 32won 40no</t>
-  </si>
-  <si>
     <t>artista</t>
   </si>
   <si>
@@ -392,144 +386,26 @@
     <t>¿? id tbc ¿?</t>
   </si>
   <si>
-    <t>import pandas as pd</t>
-  </si>
-  <si>
-    <t>import glob</t>
-  </si>
-  <si>
-    <t># Especifica el patrón de los archivos CSV que deseas unir</t>
-  </si>
-  <si>
-    <t># Obtiene la lista de archivos que coinciden con el patrón</t>
-  </si>
-  <si>
-    <t># Inicializa un DataFrame vacío para almacenar los datos combinados</t>
-  </si>
-  <si>
-    <t># Itera sobre la lista de archivos y lee cada archivo CSV en un DataFrame</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    df = pd.read_csv(file)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    # Combina el DataFrame actual con el DataFrame acumulado</t>
-  </si>
-  <si>
-    <t># Guarda el DataFrame combinado en un nuevo archivo CSV</t>
-  </si>
-  <si>
-    <t>detalles_artista  = pd.DataFrame()</t>
-  </si>
-  <si>
-    <t>detalles_artista.to_csv('detalles_artista.csv', index=False)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">pattern = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'ruta/del/directorio/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>detall_actr_*.csv'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">==&gt; todos los files que comienzan por </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>detall_actr_</t>
-    </r>
-  </si>
-  <si>
-    <t>archivos = glob.glob(pattern)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>for</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> i</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> archivos:</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">    detalles_artista = detalles_artista.append(df, index=False)</t>
-  </si>
-  <si>
-    <t>función para buscar todos los archivos que coincidan con ese patrón</t>
-  </si>
-  <si>
-    <t>limpieza código</t>
+    <t>Diseño y creación de BBDD</t>
+  </si>
+  <si>
+    <t>limpieza de código</t>
+  </si>
+  <si>
+    <t>NOMBRES DE FICHEROS ALINEADOS CON LAS TABLAS A INSERTAR EN MySQL</t>
+  </si>
+  <si>
+    <t>nombre del fichero .csv a importar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-m;@"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -680,21 +556,6 @@
       <color theme="1"/>
       <name val="Aharoni"/>
       <charset val="177"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="4"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -736,12 +597,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -752,8 +607,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -910,11 +771,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -992,63 +864,75 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1072,182 +956,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>586153</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>73269</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>21980</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>65942</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE68B825-C7B4-4E40-4656-E7F744916D53}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1802422" y="1025769"/>
-          <a:ext cx="7085135" cy="2469173"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg2">
-            <a:lumMod val="90000"/>
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-ES" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>391515</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>86508</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="A screenshot of a computer screen&#10;&#10;Description automatically generated">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FC8D1415-2DA5-E12A-B73A-B21119095231}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6705600" y="571500"/>
-          <a:ext cx="7097115" cy="5611008"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>359019</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>51289</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>549519</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>102577</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Left Brace 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5B5F4785-3347-139B-4663-3C28AFCACE1F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="359019" y="2908789"/>
-          <a:ext cx="190500" cy="1575288"/>
-        </a:xfrm>
-        <a:prstGeom prst="leftBrace">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-ES" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1293,7 +1003,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1345,7 +1055,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1539,58 +1249,60 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:AF17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AD20" sqref="AD20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="AI22" sqref="AI22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="32" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="5.140625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="19" width="4.28515625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="25" width="5.140625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="32" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="33" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:32" s="2" customFormat="1"/>
-    <row r="5" spans="2:32" s="2" customFormat="1"/>
-    <row r="6" spans="2:32" s="2" customFormat="1">
+    <row r="4" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="2:32" s="2" customFormat="1">
-      <c r="Q7" s="46" t="s">
+    <row r="7" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q7" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="47"/>
-      <c r="S7" s="47"/>
-      <c r="T7" s="47"/>
-      <c r="U7" s="47"/>
-      <c r="V7" s="47"/>
-      <c r="W7" s="47"/>
-      <c r="X7" s="47"/>
-      <c r="Y7" s="47"/>
-      <c r="Z7" s="47"/>
-      <c r="AA7" s="47"/>
-      <c r="AB7" s="47"/>
-      <c r="AC7" s="47"/>
-      <c r="AD7" s="47"/>
-      <c r="AE7" s="47"/>
-      <c r="AF7" s="47"/>
-    </row>
-    <row r="8" spans="2:32" s="2" customFormat="1" ht="15">
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="50"/>
+      <c r="U7" s="50"/>
+      <c r="V7" s="50"/>
+      <c r="W7" s="50"/>
+      <c r="X7" s="50"/>
+      <c r="Y7" s="50"/>
+      <c r="Z7" s="50"/>
+      <c r="AA7" s="50"/>
+      <c r="AB7" s="50"/>
+      <c r="AC7" s="50"/>
+      <c r="AD7" s="50"/>
+      <c r="AE7" s="50"/>
+      <c r="AF7" s="50"/>
+    </row>
+    <row r="8" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D8" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -1623,7 +1335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:32" s="2" customFormat="1">
+    <row r="9" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D9" s="5">
         <v>45224</v>
       </c>
@@ -1712,118 +1424,120 @@
         <v>45252</v>
       </c>
     </row>
-    <row r="10" spans="2:32" s="2" customFormat="1">
+    <row r="10" spans="2:32" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="55"/>
       <c r="Q10" s="24"/>
       <c r="Z10" s="24"/>
       <c r="AF10" s="25"/>
     </row>
-    <row r="11" spans="2:32" s="2" customFormat="1">
+    <row r="11" spans="2:32" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="48" t="s">
+      <c r="K11" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="49"/>
-      <c r="P11" s="49"/>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="49"/>
-      <c r="S11" s="49"/>
-      <c r="T11" s="49"/>
-      <c r="U11" s="49"/>
-      <c r="V11" s="49"/>
-      <c r="W11" s="49"/>
-      <c r="X11" s="49"/>
-      <c r="Y11" s="50"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="52"/>
+      <c r="S11" s="52"/>
+      <c r="T11" s="52"/>
+      <c r="U11" s="52"/>
+      <c r="V11" s="52"/>
+      <c r="W11" s="52"/>
+      <c r="X11" s="52"/>
+      <c r="Y11" s="53"/>
       <c r="Z11" s="24"/>
       <c r="AF11" s="25"/>
     </row>
-    <row r="12" spans="2:32" s="2" customFormat="1">
+    <row r="12" spans="2:32" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="48" t="s">
+      <c r="K12" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="49"/>
-      <c r="O12" s="49"/>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="49"/>
-      <c r="S12" s="49"/>
-      <c r="T12" s="49"/>
-      <c r="U12" s="49"/>
-      <c r="V12" s="49"/>
-      <c r="W12" s="49"/>
-      <c r="X12" s="49"/>
-      <c r="Y12" s="50"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="52"/>
+      <c r="T12" s="52"/>
+      <c r="U12" s="52"/>
+      <c r="V12" s="52"/>
+      <c r="W12" s="52"/>
+      <c r="X12" s="52"/>
+      <c r="Y12" s="53"/>
       <c r="Z12" s="24"/>
       <c r="AF12" s="25"/>
     </row>
-    <row r="13" spans="2:32" s="2" customFormat="1">
+    <row r="13" spans="2:32" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="53" t="s">
+      <c r="J13" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="54"/>
-      <c r="L13" s="55"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="58"/>
       <c r="Q13" s="24"/>
       <c r="Z13" s="24"/>
       <c r="AF13" s="25"/>
     </row>
-    <row r="14" spans="2:32" s="2" customFormat="1">
+    <row r="14" spans="2:32" s="2" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q14" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="R14" s="45"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="45"/>
-      <c r="U14" s="45"/>
-      <c r="V14" s="45"/>
-      <c r="W14" s="44"/>
+      <c r="Q14" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="R14" s="60"/>
+      <c r="S14" s="60"/>
+      <c r="T14" s="60"/>
+      <c r="U14" s="60"/>
+      <c r="V14" s="60"/>
+      <c r="W14" s="60"/>
+      <c r="X14" s="60"/>
+      <c r="Y14" s="48"/>
       <c r="Z14" s="24"/>
       <c r="AF14" s="25"/>
     </row>
-    <row r="15" spans="2:32" s="2" customFormat="1">
+    <row r="15" spans="2:32" s="2" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>5</v>
       </c>
@@ -1831,13 +1545,15 @@
         <v>16</v>
       </c>
       <c r="Q15" s="24"/>
-      <c r="Y15" s="43" t="s">
+      <c r="Y15" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="Z15" s="44"/>
+      <c r="Z15" s="65" t="s">
+        <v>17</v>
+      </c>
       <c r="AF15" s="25"/>
     </row>
-    <row r="16" spans="2:32" s="2" customFormat="1">
+    <row r="16" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>6</v>
       </c>
@@ -1845,8 +1561,8 @@
         <v>16</v>
       </c>
       <c r="Q16" s="24"/>
-      <c r="Z16" s="42" t="s">
-        <v>19</v>
+      <c r="Z16" s="39" t="s">
+        <v>18</v>
       </c>
       <c r="AA16" s="32"/>
       <c r="AB16" s="32"/>
@@ -1855,54 +1571,57 @@
       <c r="AE16" s="33"/>
       <c r="AF16" s="25"/>
     </row>
-    <row r="17" spans="3:26">
+    <row r="17" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q17" s="24"/>
-      <c r="W17" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="X17" s="45"/>
-      <c r="Y17" s="45"/>
-      <c r="Z17" s="44"/>
+      <c r="W17" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="X17" s="62"/>
+      <c r="Y17" s="62"/>
+      <c r="Z17" s="62"/>
+      <c r="AA17" s="62"/>
+      <c r="AB17" s="62"/>
+      <c r="AC17" s="62"/>
+      <c r="AD17" s="62"/>
+      <c r="AE17" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="W17:Z17"/>
-    <mergeCell ref="Q14:W14"/>
+  <mergeCells count="7">
+    <mergeCell ref="W17:AE17"/>
     <mergeCell ref="Q7:AF7"/>
     <mergeCell ref="K11:Y11"/>
     <mergeCell ref="K12:Y12"/>
     <mergeCell ref="D10:L10"/>
     <mergeCell ref="J13:L13"/>
+    <mergeCell ref="Q14:Y14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:P22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:P20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView showGridLines="0" topLeftCell="H1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="2" max="2" width="19.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="25.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="21" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="11.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="12.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="11.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
@@ -1927,410 +1646,281 @@
     <col min="33" max="33" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="19" t="s">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="I4" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="P5" s="28"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="22" t="s">
+      <c r="J6" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="P5" s="28"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="16" t="s">
+      <c r="I8" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="62" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="17" t="s">
+      <c r="C9" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="N9" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="21" t="s">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I10" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="61" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="N9" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="O9" s="37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="I10" s="21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="21" t="s">
+      <c r="B11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="C11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="I11" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="J11" s="27" t="s">
-        <v>50</v>
-      </c>
       <c r="K11" s="37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C12" s="29"/>
       <c r="D12" s="30"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I13" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="23"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I16" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="K17" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="M17" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="N17" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="40"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="J20" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="L20" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="M20" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="O20" s="36" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14" s="59" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="B15" s="23"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="I16" s="21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="J17" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="K17" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="L17" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="M17" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="N17" s="34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1">
-      <c r="C18" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" s="57"/>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="C19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="C20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="A22" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="J22" s="60" t="s">
-        <v>74</v>
-      </c>
-      <c r="K22" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="L22" s="63" t="s">
-        <v>76</v>
-      </c>
-      <c r="M22" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="O22" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="F18:G20"/>
+  <mergeCells count="1">
+    <mergeCell ref="A4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B6:H26"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="6" spans="2:7">
-      <c r="B6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="39"/>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="C8" s="41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="C9" s="41"/>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="D12" s="40" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="36"/>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="B25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>